<commit_message>
Added wing loadings at cruise and landing
</commit_message>
<xml_diff>
--- a/Performance analysis/inputs_outputs.xlsx
+++ b/Performance analysis/inputs_outputs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4280" yWindow="460" windowWidth="28040" windowHeight="16280" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16280" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inputs" sheetId="1" state="visible" r:id="rId1"/>
@@ -359,8 +359,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -408,7 +408,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>class 1 (needs to be updated)</t>
+          <t>class 1</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
         </is>
       </c>
       <c r="B3">
-        <f>1858+6981</f>
+        <f>8839</f>
         <v/>
       </c>
       <c r="C3" t="inlineStr">
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="B4">
-        <f>190*1000/3600</f>
+        <f>52.778</f>
         <v/>
       </c>
       <c r="C4" t="inlineStr">
@@ -655,17 +655,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col width="20.83203125" customWidth="1" min="1" max="1"/>
     <col width="13.83203125" customWidth="1" min="2" max="2"/>
-    <col width="20.5" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -706,7 +706,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Wing loading diagra</t>
+          <t>Wing loading diagram</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Wing loading diagra</t>
+          <t>Wing loading diagram</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,47 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Wing loading diagra</t>
+          <t>Wing loading diagram</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Wing loading at cruise</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4405.636769211125</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>N/m^2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Wing loading diagram</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Wing loading at landing</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4872.47953908665</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>N/m^2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Wing loading diagram</t>
         </is>
       </c>
     </row>

</xml_diff>